<commit_message>
Removes 0 Nov 2016
</commit_message>
<xml_diff>
--- a/static/downloads/production/monthly_production.xlsx
+++ b/static/downloads/production/monthly_production.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faiedm\Documents\GitHub\nrrd\static\downloads\production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35322E85-D525-41BC-818E-699983D08C3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15979438-115A-4002-81CC-03E63398459C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="255" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6598" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6599" uniqueCount="26">
   <si>
     <t>Month</t>
   </si>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1649"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A470" workbookViewId="0">
-      <selection activeCell="C477" sqref="C477"/>
+    <sheetView tabSelected="1" topLeftCell="A1319" workbookViewId="0">
+      <selection activeCell="D1332" sqref="D1332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -27196,8 +27196,8 @@
       <c r="C1331" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D1331" s="12">
-        <v>0</v>
+      <c r="D1331" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="E1331" s="12" t="s">
         <v>9</v>

</xml_diff>